<commit_message>
update scripts and result from scripts
</commit_message>
<xml_diff>
--- a/study01/report/motivation/scr-effective-participants/effort-importance/by-Type/NonParametricAnalysis.xlsx
+++ b/study01/report/motivation/scr-effective-participants/effort-importance/by-Type/NonParametricAnalysis.xlsx
@@ -12907,13 +12907,13 @@
         <v>208.5</v>
       </c>
       <c r="G7" t="n" s="257">
-        <v>-1.504474196358279</v>
+        <v>-1.5044741963582788</v>
       </c>
       <c r="H7" t="n" s="258">
         <v>0.06739702170622115</v>
       </c>
       <c r="I7" t="n" s="259">
-        <v>0.21715214556407458</v>
+        <v>0.21715214556407456</v>
       </c>
       <c r="J7" t="s" s="260">
         <v>48</v>
@@ -12939,13 +12939,13 @@
         <v>208.5</v>
       </c>
       <c r="G8" t="n" s="257">
-        <v>-1.504474196358279</v>
+        <v>-1.5044741963582788</v>
       </c>
       <c r="H8" t="n" s="258">
         <v>0.06739702170622115</v>
       </c>
       <c r="I8" t="n" s="259">
-        <v>0.21715214556407458</v>
+        <v>0.21715214556407456</v>
       </c>
       <c r="J8" t="s" s="260">
         <v>48</v>
@@ -13008,13 +13008,13 @@
         <v>208.5</v>
       </c>
       <c r="G11" t="n" s="285">
-        <v>-1.504474196358279</v>
+        <v>-1.5044741963582788</v>
       </c>
       <c r="H11" t="n" s="286">
         <v>0.9339771082414066</v>
       </c>
       <c r="I11" t="n" s="287">
-        <v>0.21715214556407458</v>
+        <v>0.21715214556407456</v>
       </c>
       <c r="J11" t="s" s="288">
         <v>48</v>
@@ -13040,13 +13040,13 @@
         <v>208.5</v>
       </c>
       <c r="G12" t="n" s="285">
-        <v>-1.504474196358279</v>
+        <v>-1.5044741963582788</v>
       </c>
       <c r="H12" t="n" s="286">
         <v>0.9339771082414066</v>
       </c>
       <c r="I12" t="n" s="287">
-        <v>0.21715214556407458</v>
+        <v>0.21715214556407456</v>
       </c>
       <c r="J12" t="s" s="288">
         <v>48</v>
@@ -13109,13 +13109,13 @@
         <v>208.5</v>
       </c>
       <c r="G15" t="n" s="313">
-        <v>-1.504474196358279</v>
+        <v>-1.5044741963582788</v>
       </c>
       <c r="H15" t="n" s="314">
         <v>0.13480618126956417</v>
       </c>
       <c r="I15" t="n" s="315">
-        <v>0.21715214556407458</v>
+        <v>0.21715214556407456</v>
       </c>
       <c r="J15" t="s" s="316">
         <v>48</v>
@@ -13141,13 +13141,13 @@
         <v>208.5</v>
       </c>
       <c r="G16" t="n" s="313">
-        <v>-1.504474196358279</v>
+        <v>-1.5044741963582788</v>
       </c>
       <c r="H16" t="n" s="314">
         <v>0.13480618126956417</v>
       </c>
       <c r="I16" t="n" s="315">
-        <v>0.21715214556407458</v>
+        <v>0.21715214556407456</v>
       </c>
       <c r="J16" t="s" s="316">
         <v>48</v>
@@ -31421,13 +31421,13 @@
         <v>109.5</v>
       </c>
       <c r="G7" t="n" s="1259">
-        <v>0.5343541567906561</v>
+        <v>0.534354156790656</v>
       </c>
       <c r="H7" t="n" s="1260">
         <v>0.7049012129642094</v>
       </c>
       <c r="I7" t="n" s="1261">
-        <v>0.10098344363583515</v>
+        <v>0.10098344363583514</v>
       </c>
       <c r="J7" t="s" s="1262">
         <v>48</v>
@@ -31453,13 +31453,13 @@
         <v>109.5</v>
       </c>
       <c r="G8" t="n" s="1259">
-        <v>0.5343541567906561</v>
+        <v>0.534354156790656</v>
       </c>
       <c r="H8" t="n" s="1260">
         <v>0.7049012129642094</v>
       </c>
       <c r="I8" t="n" s="1261">
-        <v>0.10098344363583515</v>
+        <v>0.10098344363583514</v>
       </c>
       <c r="J8" t="s" s="1262">
         <v>48</v>
@@ -31522,13 +31522,13 @@
         <v>109.5</v>
       </c>
       <c r="G11" t="n" s="1287">
-        <v>0.5343541567906561</v>
+        <v>0.534354156790656</v>
       </c>
       <c r="H11" t="n" s="1288">
         <v>0.3037280327844334</v>
       </c>
       <c r="I11" t="n" s="1289">
-        <v>0.10098344363583515</v>
+        <v>0.10098344363583514</v>
       </c>
       <c r="J11" t="s" s="1290">
         <v>48</v>
@@ -31554,13 +31554,13 @@
         <v>109.5</v>
       </c>
       <c r="G12" t="n" s="1287">
-        <v>0.5343541567906561</v>
+        <v>0.534354156790656</v>
       </c>
       <c r="H12" t="n" s="1288">
         <v>0.3037280327844334</v>
       </c>
       <c r="I12" t="n" s="1289">
-        <v>0.10098344363583515</v>
+        <v>0.10098344363583514</v>
       </c>
       <c r="J12" t="s" s="1290">
         <v>48</v>
@@ -31623,13 +31623,13 @@
         <v>109.5</v>
       </c>
       <c r="G15" t="n" s="1315">
-        <v>0.5343541567906561</v>
+        <v>0.534354156790656</v>
       </c>
       <c r="H15" t="n" s="1316">
         <v>0.6074560655688668</v>
       </c>
       <c r="I15" t="n" s="1317">
-        <v>0.10098344363583515</v>
+        <v>0.10098344363583514</v>
       </c>
       <c r="J15" t="s" s="1318">
         <v>48</v>
@@ -31655,13 +31655,13 @@
         <v>109.5</v>
       </c>
       <c r="G16" t="n" s="1315">
-        <v>0.5343541567906561</v>
+        <v>0.534354156790656</v>
       </c>
       <c r="H16" t="n" s="1316">
         <v>0.6074560655688668</v>
       </c>
       <c r="I16" t="n" s="1317">
-        <v>0.10098344363583515</v>
+        <v>0.10098344363583514</v>
       </c>
       <c r="J16" t="s" s="1318">
         <v>48</v>

</xml_diff>